<commit_message>
Added more data tables in csv_exports, updated README, added project-update.md
</commit_message>
<xml_diff>
--- a/data/tracking_data_processing.xlsx
+++ b/data/tracking_data_processing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/T7/Data_Viz/Final_Project/noah-baustin/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF726E44-3703-7D4F-A5D5-5C62375DF6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C0D6E8-A312-0242-9A30-DB373DB8BF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38480" yWindow="500" windowWidth="36780" windowHeight="17440" activeTab="1" xr2:uid="{27FC8F3F-5E1E-5D4E-B377-3BFE9D915A76}"/>
+    <workbookView xWindow="47840" yWindow="500" windowWidth="26220" windowHeight="17440" xr2:uid="{27FC8F3F-5E1E-5D4E-B377-3BFE9D915A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>CA number of felony marijuana arrests</t>
   </si>
@@ -68,6 +68,24 @@
   </si>
   <si>
     <t>Duplicated all the pdfs into a new folder where I can edit them to the pages I need: /Volumes/T7/Data_Viz/Final_Project/noah-baustin/data/edited_pdfs</t>
+  </si>
+  <si>
+    <t>ca_felony_arrests_2015-2020</t>
+  </si>
+  <si>
+    <t>ca_misdemeanor_arrests_offense_by_gender_and_race_ethnic_group_2020</t>
+  </si>
+  <si>
+    <t>ca_misdeamnor_arrests_.by_offense_for_adult_and_juvenile_arrests</t>
+  </si>
+  <si>
+    <t>felony_arrests_category_and_offense_by_age_group_of_arrestee_2020</t>
+  </si>
+  <si>
+    <t>misdemeanor_arrests_offense_by_age_group_of_arrestee_2020.csv</t>
+  </si>
+  <si>
+    <t>felony_arrests_category_and_offense_by_gender_and_race_ethnic_group_of_arrestee._2020.csv</t>
   </si>
 </sst>
 </file>
@@ -437,20 +455,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824C7DDA-D05B-0A43-8866-E8044EFD84B5}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="37.5" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
     <col min="6" max="6" width="40.1640625" customWidth="1"/>
     <col min="7" max="7" width="45.83203125" customWidth="1"/>
-    <col min="8" max="8" width="42" customWidth="1"/>
+    <col min="8" max="8" width="45.1640625" customWidth="1"/>
     <col min="9" max="9" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -484,30 +503,84 @@
       <c r="A2" s="2">
         <v>2020</v>
       </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2019</v>
       </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2018</v>
       </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2016</v>
       </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2015</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -644,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957C2947-BF5C-8244-9D78-D4630A739BB5}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+    <sheetView zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>